<commit_message>
Add -TdP to keys with TdP in Cipa file
</commit_message>
<xml_diff>
--- a/CiPA28.xlsx
+++ b/CiPA28.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upvedues-my.sharepoint.com/personal/mamofe_upv_edu_es/Documents/POSTDOC/Proyectos/SimCardioTest/Simula/7-ecg/Sent/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/finsberg/local/src/reproduce-ecg-upv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{027CD972-A636-4DB0-ACD4-5B1392EE6B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A264A3E9-8FA3-4E4C-937D-72D5EEB2405F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B6A126-D11D-0A4D-90F3-8A62F780037C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-1270" windowWidth="19420" windowHeight="11500" xr2:uid="{2505763F-C0DE-45D9-9152-C347D67BEC19}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{2505763F-C0DE-45D9-9152-C347D67BEC19}"/>
   </bookViews>
   <sheets>
     <sheet name="fraction" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="63">
   <si>
     <t>Sotalol</t>
   </si>
@@ -225,6 +224,12 @@
   </si>
   <si>
     <t>TdP</t>
+  </si>
+  <si>
+    <t>Quinidine-TdP</t>
+  </si>
+  <si>
+    <t>Clozapine-TdP</t>
   </si>
 </sst>
 </file>
@@ -418,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -509,20 +514,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -530,7 +524,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="1" builtinId="10"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -546,9 +540,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -586,7 +580,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -692,7 +686,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -834,7 +828,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -844,23 +838,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AA3245-A2F9-47AC-BC55-B58C081B6EC1}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="16" width="11.42578125" style="6"/>
-    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="16" width="11.5" style="6"/>
+    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B1" s="26" t="s">
         <v>54</v>
       </c>
@@ -903,7 +897,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
         <v>58</v>
       </c>
@@ -944,8 +938,8 @@
       <c r="S2" s="42"/>
       <c r="T2" s="43"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B3">
@@ -969,8 +963,8 @@
       <c r="S3" s="33"/>
       <c r="T3" s="34"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B4">
@@ -1002,8 +996,8 @@
       <c r="S4" s="33"/>
       <c r="T4" s="34"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="7">
@@ -1039,8 +1033,8 @@
       <c r="S5" s="33"/>
       <c r="T5" s="33"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B6">
@@ -1080,8 +1074,8 @@
       <c r="S6" s="33"/>
       <c r="T6" s="34"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="8">
@@ -1121,8 +1115,8 @@
       <c r="S7" s="33"/>
       <c r="T7" s="34"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B8">
@@ -1150,8 +1144,8 @@
       <c r="S8" s="33"/>
       <c r="T8" s="33"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="8">
@@ -1179,8 +1173,8 @@
       <c r="S9" s="33"/>
       <c r="T9" s="34"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B10">
@@ -1216,8 +1210,8 @@
       <c r="S10" s="33"/>
       <c r="T10" s="34"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B11">
@@ -1245,8 +1239,8 @@
       <c r="S11" s="33"/>
       <c r="T11" s="34"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="8">
@@ -1282,8 +1276,8 @@
       <c r="S12" s="33"/>
       <c r="T12" s="34"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B13">
@@ -1311,8 +1305,8 @@
       <c r="S13" s="33"/>
       <c r="T13" s="34"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="50" t="s">
+    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
         <v>26</v>
       </c>
       <c r="B14">
@@ -1336,8 +1330,8 @@
       <c r="S14" s="33"/>
       <c r="T14" s="34"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="7">
@@ -1365,8 +1359,8 @@
       <c r="S15" s="33"/>
       <c r="T15" s="33"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="7">
@@ -1394,8 +1388,8 @@
       <c r="S16" s="33"/>
       <c r="T16" s="34"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
         <v>55</v>
       </c>
       <c r="B17">
@@ -1423,8 +1417,8 @@
       <c r="S17" s="33"/>
       <c r="T17" s="34"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B18">
@@ -1452,8 +1446,8 @@
       <c r="S18" s="33"/>
       <c r="T18" s="34"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="7">
@@ -1485,8 +1479,8 @@
       <c r="S19" s="35"/>
       <c r="T19" s="36"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="7">
@@ -1514,8 +1508,8 @@
       <c r="S20" s="33"/>
       <c r="T20" s="33"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
+    <row r="21" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="8">
@@ -1551,8 +1545,8 @@
       <c r="S21" s="33"/>
       <c r="T21" s="34"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+    <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B22">
@@ -1584,8 +1578,8 @@
       <c r="S22" s="33"/>
       <c r="T22" s="34"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
+    <row r="23" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B23">
@@ -1625,8 +1619,8 @@
       <c r="S23" s="33"/>
       <c r="T23" s="34"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="7">
@@ -1662,8 +1656,8 @@
       <c r="S24" s="33"/>
       <c r="T24" s="34"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="48" t="s">
+    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="7">
@@ -1696,8 +1690,8 @@
       <c r="S25" s="33"/>
       <c r="T25" s="34"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="8">
@@ -1734,8 +1728,8 @@
       <c r="S26" s="33"/>
       <c r="T26" s="34"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="47" t="s">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B27">
@@ -1752,8 +1746,8 @@
       <c r="S27" s="33"/>
       <c r="T27" s="34"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+    <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="7">
@@ -1790,8 +1784,8 @@
       <c r="S28" s="33"/>
       <c r="T28" s="34"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
         <v>35</v>
       </c>
       <c r="B29">
@@ -1808,8 +1802,8 @@
       <c r="S29" s="33"/>
       <c r="T29" s="34"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="7">
@@ -1850,14 +1844,14 @@
       <c r="S30" s="33"/>
       <c r="T30" s="34"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="52" t="s">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="47" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
-        <v>31</v>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="48" t="s">
+        <v>61</v>
       </c>
       <c r="B35">
         <f>'IC50'!B35</f>
@@ -1892,11 +1886,11 @@
         <v>0.55451551299111113</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="51">
+    <row r="36" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="7">
         <f>'IC50'!B36*10</f>
         <v>1535.0649524812775</v>
       </c>
@@ -1927,19 +1921,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED62F087-9FE5-4C8B-92F3-BA311049ACFA}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1986,7 +1980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>39</v>
       </c>
@@ -2012,7 +2006,7 @@
         <v>2.0960000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -2050,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
@@ -2094,7 +2088,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>18</v>
       </c>
@@ -2144,7 +2138,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>19</v>
       </c>
@@ -2194,7 +2188,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>20</v>
       </c>
@@ -2226,7 +2220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>21</v>
       </c>
@@ -2258,7 +2252,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>22</v>
       </c>
@@ -2302,7 +2296,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>23</v>
       </c>
@@ -2340,7 +2334,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>24</v>
       </c>
@@ -2384,7 +2378,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>25</v>
       </c>
@@ -2431,7 +2425,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>26</v>
       </c>
@@ -2459,7 +2453,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>38</v>
       </c>
@@ -2491,7 +2485,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>27</v>
       </c>
@@ -2523,7 +2517,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>55</v>
       </c>
@@ -2555,7 +2549,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>28</v>
       </c>
@@ -2605,7 +2599,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>1</v>
       </c>
@@ -2643,7 +2637,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>41</v>
       </c>
@@ -2675,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>29</v>
       </c>
@@ -2725,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>30</v>
       </c>
@@ -2772,7 +2766,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>31</v>
       </c>
@@ -2822,7 +2816,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>32</v>
       </c>
@@ -2866,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
         <v>33</v>
       </c>
@@ -2904,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>0</v>
       </c>
@@ -2948,7 +2942,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>34</v>
       </c>
@@ -2967,7 +2961,7 @@
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>40</v>
       </c>
@@ -3011,7 +3005,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
         <v>35</v>
       </c>
@@ -3045,7 +3039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>42</v>
       </c>
@@ -3095,14 +3089,14 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="45" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B35">
         <v>2946.5419470220563</v>
@@ -3150,9 +3144,9 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B36">
         <v>153.50649524812775</v>
@@ -3199,7 +3193,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3213,59 +3207,59 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>28.3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>22.9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>39.9</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>0.33200000000000002</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>2.62</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>1.4088000000000001</v>
       </c>
@@ -3274,32 +3268,32 @@
         <v>1.639</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>1.3951</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>2.5186999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>1.589</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>1.2257</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>1.639</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>5.4843999999999997E-2</v>
       </c>
@@ -3310,6 +3304,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fd20df89-4048-49a6-a67a-390eaa975cff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006E43017B494BB149B6A2335A5C790C9A" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="506d71b03f66a101d5518de95d44f535">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fd20df89-4048-49a6-a67a-390eaa975cff" xmlns:ns4="92ab9642-0aab-44de-b012-9f00b4c0dc56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1061fe56412549e533d1e88f97579ff" ns3:_="" ns4:_="">
     <xsd:import namespace="fd20df89-4048-49a6-a67a-390eaa975cff"/>
@@ -3556,38 +3567,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fd20df89-4048-49a6-a67a-390eaa975cff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{410EA7CD-8428-4838-8AA2-CE3DCE6A747C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66B0185D-0079-420A-8018-4117B6CFA962}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fd20df89-4048-49a6-a67a-390eaa975cff"/>
-    <ds:schemaRef ds:uri="92ab9642-0aab-44de-b012-9f00b4c0dc56"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3610,9 +3593,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66B0185D-0079-420A-8018-4117B6CFA962}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{410EA7CD-8428-4838-8AA2-CE3DCE6A747C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fd20df89-4048-49a6-a67a-390eaa975cff"/>
+    <ds:schemaRef ds:uri="92ab9642-0aab-44de-b012-9f00b4c0dc56"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Use _ in TdP
</commit_message>
<xml_diff>
--- a/CiPA28.xlsx
+++ b/CiPA28.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/finsberg/local/src/reproduce-ecg-upv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B6A126-D11D-0A4D-90F3-8A62F780037C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDAC6BD-712C-A344-AB42-07C849B32571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{2505763F-C0DE-45D9-9152-C347D67BEC19}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{2505763F-C0DE-45D9-9152-C347D67BEC19}"/>
   </bookViews>
   <sheets>
     <sheet name="fraction" sheetId="4" r:id="rId1"/>
@@ -226,10 +226,10 @@
     <t>TdP</t>
   </si>
   <si>
-    <t>Quinidine-TdP</t>
-  </si>
-  <si>
-    <t>Clozapine-TdP</t>
+    <t>Quinidine_TdP</t>
+  </si>
+  <si>
+    <t>Clozapine_TdP</t>
   </si>
 </sst>
 </file>
@@ -838,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AA3245-A2F9-47AC-BC55-B58C081B6EC1}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1921,7 +1921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED62F087-9FE5-4C8B-92F3-BA311049ACFA}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3313,14 +3313,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fd20df89-4048-49a6-a67a-390eaa975cff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006E43017B494BB149B6A2335A5C790C9A" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="506d71b03f66a101d5518de95d44f535">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fd20df89-4048-49a6-a67a-390eaa975cff" xmlns:ns4="92ab9642-0aab-44de-b012-9f00b4c0dc56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1061fe56412549e533d1e88f97579ff" ns3:_="" ns4:_="">
     <xsd:import namespace="fd20df89-4048-49a6-a67a-390eaa975cff"/>
@@ -3567,6 +3559,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fd20df89-4048-49a6-a67a-390eaa975cff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66B0185D-0079-420A-8018-4117B6CFA962}">
   <ds:schemaRefs>
@@ -3576,23 +3576,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13E2453B-FDCB-4FD8-976D-FFA0386AE37D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="92ab9642-0aab-44de-b012-9f00b4c0dc56"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="fd20df89-4048-49a6-a67a-390eaa975cff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{410EA7CD-8428-4838-8AA2-CE3DCE6A747C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3609,4 +3592,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13E2453B-FDCB-4FD8-976D-FFA0386AE37D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="92ab9642-0aab-44de-b012-9f00b4c0dc56"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="fd20df89-4048-49a6-a67a-390eaa975cff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>